<commit_message>
Added basic program for fish cut
</commit_message>
<xml_diff>
--- a/cut_program_output/FishyFish_0.xlsx
+++ b/cut_program_output/FishyFish_0.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="6">
   <si>
     <t>Feed</t>
+  </si>
+  <si>
+    <t>V-Axis</t>
   </si>
   <si>
     <t>Operation</t>
@@ -386,1118 +389,1421 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1040</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1040</v>
       </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
         <v>1040</v>
       </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
         <v>1040</v>
       </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
         <v>235</v>
       </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
         <v>805</v>
       </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
         <v>195</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11">
         <v>825</v>
       </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12">
         <v>175</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14">
         <v>845</v>
       </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15">
         <v>155</v>
       </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16">
         <v>20</v>
       </c>
-      <c r="C16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17">
         <v>865</v>
       </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18">
         <v>135</v>
       </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20">
         <v>885</v>
       </c>
-      <c r="C20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21">
         <v>115</v>
       </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22">
         <v>120</v>
       </c>
-      <c r="C22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23">
         <v>805</v>
       </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24">
         <v>195</v>
       </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25">
         <v>20</v>
       </c>
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26">
         <v>825</v>
       </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27">
         <v>175</v>
       </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28">
         <v>20</v>
       </c>
-      <c r="C28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29">
         <v>845</v>
       </c>
-      <c r="C29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="C29">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30">
         <v>155</v>
       </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31">
         <v>20</v>
       </c>
-      <c r="C31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32">
         <v>865</v>
       </c>
-      <c r="C32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33">
         <v>135</v>
       </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34">
         <v>20</v>
       </c>
-      <c r="C34" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35">
         <v>885</v>
       </c>
-      <c r="C35" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="C35">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36">
         <v>115</v>
       </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37">
         <v>120</v>
       </c>
-      <c r="C37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38">
         <v>805</v>
       </c>
-      <c r="C38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="C38">
+        <v>20</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39">
         <v>195</v>
       </c>
-      <c r="C39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40">
         <v>20</v>
       </c>
-      <c r="C40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41">
         <v>825</v>
       </c>
-      <c r="C41" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="C41">
+        <v>20</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42">
         <v>175</v>
       </c>
-      <c r="C42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43">
         <v>20</v>
       </c>
-      <c r="C43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44">
         <v>845</v>
       </c>
-      <c r="C44" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="C44">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45">
         <v>155</v>
       </c>
-      <c r="C45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46">
         <v>20</v>
       </c>
-      <c r="C46" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47">
         <v>865</v>
       </c>
-      <c r="C47" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="C47">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48">
         <v>135</v>
       </c>
-      <c r="C48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49">
         <v>20</v>
       </c>
-      <c r="C49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50">
         <v>885</v>
       </c>
-      <c r="C50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="C50">
+        <v>20</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51">
         <v>115</v>
       </c>
-      <c r="C51" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52">
         <v>120</v>
       </c>
-      <c r="C52" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53">
         <v>805</v>
       </c>
-      <c r="C53" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="C53">
+        <v>20</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54">
         <v>195</v>
       </c>
-      <c r="C54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55">
         <v>20</v>
       </c>
-      <c r="C55" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56">
         <v>825</v>
       </c>
-      <c r="C56" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="C56">
+        <v>20</v>
+      </c>
+      <c r="D56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57">
         <v>175</v>
       </c>
-      <c r="C57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58">
         <v>20</v>
       </c>
-      <c r="C58" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59">
         <v>845</v>
       </c>
-      <c r="C59" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="C59">
+        <v>20</v>
+      </c>
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60">
         <v>155</v>
       </c>
-      <c r="C60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61">
         <v>20</v>
       </c>
-      <c r="C61" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62">
         <v>865</v>
       </c>
-      <c r="C62" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63">
         <v>135</v>
       </c>
-      <c r="C63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64">
         <v>20</v>
       </c>
-      <c r="C64" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65">
         <v>885</v>
       </c>
-      <c r="C65" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="C65">
+        <v>20</v>
+      </c>
+      <c r="D65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66">
         <v>115</v>
       </c>
-      <c r="C66" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67">
         <v>120</v>
       </c>
-      <c r="C67" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68">
         <v>805</v>
       </c>
-      <c r="C68" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="C68">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69">
         <v>195</v>
       </c>
-      <c r="C69" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70">
         <v>20</v>
       </c>
-      <c r="C70" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71">
         <v>825</v>
       </c>
-      <c r="C71" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="C71">
+        <v>20</v>
+      </c>
+      <c r="D71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72">
         <v>175</v>
       </c>
-      <c r="C72" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="1">
         <v>72</v>
       </c>
       <c r="B73">
         <v>20</v>
       </c>
-      <c r="C73" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="1">
         <v>73</v>
       </c>
       <c r="B74">
         <v>845</v>
       </c>
-      <c r="C74" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="C74">
+        <v>20</v>
+      </c>
+      <c r="D74" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="1">
         <v>74</v>
       </c>
       <c r="B75">
         <v>155</v>
       </c>
-      <c r="C75" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="B76">
         <v>20</v>
       </c>
-      <c r="C76" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="1">
         <v>76</v>
       </c>
       <c r="B77">
         <v>865</v>
       </c>
-      <c r="C77" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="C77">
+        <v>20</v>
+      </c>
+      <c r="D77" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78">
         <v>135</v>
       </c>
-      <c r="C78" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="1">
         <v>78</v>
       </c>
       <c r="B79">
         <v>20</v>
       </c>
-      <c r="C79" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="1">
         <v>79</v>
       </c>
       <c r="B80">
         <v>885</v>
       </c>
-      <c r="C80" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="C80">
+        <v>20</v>
+      </c>
+      <c r="D80" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81">
         <v>115</v>
       </c>
-      <c r="C81" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="1">
         <v>81</v>
       </c>
       <c r="B82">
         <v>120</v>
       </c>
-      <c r="C82" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="1">
         <v>82</v>
       </c>
       <c r="B83">
         <v>805</v>
       </c>
-      <c r="C83" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="C83">
+        <v>20</v>
+      </c>
+      <c r="D83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84">
         <v>195</v>
       </c>
-      <c r="C84" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="1">
         <v>84</v>
       </c>
       <c r="B85">
         <v>20</v>
       </c>
-      <c r="C85" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="1">
         <v>85</v>
       </c>
       <c r="B86">
         <v>825</v>
       </c>
-      <c r="C86" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="C86">
+        <v>20</v>
+      </c>
+      <c r="D86" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="1">
         <v>86</v>
       </c>
       <c r="B87">
         <v>175</v>
       </c>
-      <c r="C87" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88">
         <v>20</v>
       </c>
-      <c r="C88" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="1">
         <v>88</v>
       </c>
       <c r="B89">
         <v>845</v>
       </c>
-      <c r="C89" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="C89">
+        <v>20</v>
+      </c>
+      <c r="D89" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="1">
         <v>89</v>
       </c>
       <c r="B90">
         <v>155</v>
       </c>
-      <c r="C90" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="1">
         <v>90</v>
       </c>
       <c r="B91">
         <v>20</v>
       </c>
-      <c r="C91" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="1">
         <v>91</v>
       </c>
       <c r="B92">
         <v>865</v>
       </c>
-      <c r="C92" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="C92">
+        <v>20</v>
+      </c>
+      <c r="D92" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" s="1">
         <v>92</v>
       </c>
       <c r="B93">
         <v>135</v>
       </c>
-      <c r="C93" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="1">
         <v>93</v>
       </c>
       <c r="B94">
         <v>20</v>
       </c>
-      <c r="C94" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="1">
         <v>94</v>
       </c>
       <c r="B95">
         <v>885</v>
       </c>
-      <c r="C95" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="C95">
+        <v>20</v>
+      </c>
+      <c r="D95" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="1">
         <v>95</v>
       </c>
       <c r="B96">
         <v>115</v>
       </c>
-      <c r="C96" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="1">
         <v>96</v>
       </c>
       <c r="B97">
         <v>120</v>
       </c>
-      <c r="C97" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="1">
         <v>97</v>
       </c>
       <c r="B98">
         <v>805</v>
       </c>
-      <c r="C98" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="C98">
+        <v>20</v>
+      </c>
+      <c r="D98" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="1">
         <v>98</v>
       </c>
       <c r="B99">
         <v>195</v>
       </c>
-      <c r="C99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="1">
         <v>99</v>
       </c>
       <c r="B100">
         <v>20</v>
       </c>
-      <c r="C100" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="1">
         <v>100</v>
       </c>
       <c r="B101">
         <v>825</v>
       </c>
-      <c r="C101" t="s">
-        <v>2</v>
+      <c r="C101">
+        <v>20</v>
+      </c>
+      <c r="D101" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>